<commit_message>
started making relative data, fixed bug in plotly bar plot that gets broken when there are negative values
</commit_message>
<xml_diff>
--- a/data/statistika u nizu/Stanovnistvo.xlsx
+++ b/data/statistika u nizu/Stanovnistvo.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="132" yWindow="-192" windowWidth="23052" windowHeight="14316"/>
+    <workbookView xWindow="135" yWindow="-195" windowWidth="23055" windowHeight="14310" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sadržaj-Contents" sheetId="1" r:id="rId1"/>
-    <sheet name="7.2.1." sheetId="4" r:id="rId2"/>
-    <sheet name="7.2.2." sheetId="5" r:id="rId3"/>
-    <sheet name="7.2.3." sheetId="6" r:id="rId4"/>
+    <sheet name="7.4.1." sheetId="4" r:id="rId2"/>
+    <sheet name="7.4.2." sheetId="5" r:id="rId3"/>
+    <sheet name="7.4.3." sheetId="6" r:id="rId4"/>
     <sheet name="Metodološka objašnjenja" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -1260,24 +1260,6 @@
     <t>PROCJENA UKUPNOG BROJA STANOVNIKA SREDINOM GODINE</t>
   </si>
   <si>
-    <t>7.2.1.</t>
-  </si>
-  <si>
-    <t>7.2.2.</t>
-  </si>
-  <si>
-    <t>7.2.3.</t>
-  </si>
-  <si>
-    <t>Tab. 7.2.1.</t>
-  </si>
-  <si>
-    <t>Tab. 7.2.2.</t>
-  </si>
-  <si>
-    <t>Tab. 7.2.3.</t>
-  </si>
-  <si>
     <t>2015.</t>
   </si>
   <si>
@@ -1342,6 +1324,24 @@
       </rPr>
       <t xml:space="preserve">have been calculated on the basis of the 2011 Census, natural change and net migration data. </t>
     </r>
+  </si>
+  <si>
+    <t>Tab. 7.4.1.</t>
+  </si>
+  <si>
+    <t>7.4.1.</t>
+  </si>
+  <si>
+    <t>7.4.2.</t>
+  </si>
+  <si>
+    <t>Tab. 7.4.2.</t>
+  </si>
+  <si>
+    <t>7.4.3.</t>
+  </si>
+  <si>
+    <t>Tab. 7.4.3.</t>
   </si>
 </sst>
 </file>
@@ -2329,6 +2329,12 @@
     <xf numFmtId="3" fontId="14" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" wrapText="1"/>
       <protection locked="0"/>
@@ -2342,12 +2348,6 @@
     </xf>
     <xf numFmtId="3" fontId="13" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
@@ -2943,11 +2943,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:18" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="84"/>
@@ -2957,7 +2957,7 @@
       <c r="E1" s="86"/>
       <c r="F1" s="87"/>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>96</v>
       </c>
@@ -2966,7 +2966,7 @@
       <c r="D2" s="5"/>
       <c r="E2" s="6"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>97</v>
       </c>
@@ -2975,7 +2975,7 @@
       <c r="D3" s="5"/>
       <c r="E3" s="6"/>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>0</v>
       </c>
@@ -2984,7 +2984,7 @@
       <c r="D4" s="83"/>
       <c r="E4" s="6"/>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>1</v>
       </c>
@@ -2993,9 +2993,9 @@
       <c r="D5" s="6"/>
       <c r="E5" s="6"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="137" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="C7" s="104" t="s">
         <v>113</v>
@@ -3008,7 +3008,7 @@
       <c r="I7" s="103"/>
       <c r="J7" s="103"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="12"/>
       <c r="C8" s="106" t="s">
         <v>114</v>
@@ -3021,9 +3021,9 @@
       <c r="I8" s="103"/>
       <c r="J8" s="103"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="137" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="C9" s="104" t="s">
         <v>115</v>
@@ -3036,7 +3036,7 @@
       <c r="I9" s="103"/>
       <c r="J9" s="103"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="12"/>
       <c r="C10" s="106" t="s">
         <v>116</v>
@@ -3049,9 +3049,9 @@
       <c r="I10" s="103"/>
       <c r="J10" s="103"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="137" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="C11" s="104" t="s">
         <v>172</v>
@@ -3064,7 +3064,7 @@
       <c r="I11" s="103"/>
       <c r="J11" s="103"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="12"/>
       <c r="C12" s="106" t="s">
         <v>151</v>
@@ -3077,7 +3077,7 @@
       <c r="I12" s="103"/>
       <c r="J12" s="103"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="12"/>
       <c r="C13" s="138" t="s">
         <v>98</v>
@@ -3098,7 +3098,7 @@
       <c r="Q13" s="17"/>
       <c r="R13" s="17"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C14" s="139" t="s">
         <v>112</v>
       </c>
@@ -3118,28 +3118,28 @@
       <c r="Q14" s="17"/>
       <c r="R14" s="17"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C15" s="1"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C16" s="20"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="3:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C17" s="1"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
       <c r="F17" s="3"/>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="3:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="3:7" ht="14.45" x14ac:dyDescent="0.3">
       <c r="C18" s="7"/>
       <c r="D18" s="4"/>
       <c r="E18" s="4"/>
@@ -3148,11 +3148,11 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A7" location="'7.2.1.'!A1" display="Tab. 7.2.1."/>
-    <hyperlink ref="A9" location="'7.2.2.'!A1" display="Tab. 3.2."/>
-    <hyperlink ref="A11" location="'7.2.3.'!A1" display="Tab. 3.3."/>
     <hyperlink ref="C13" location="'Metodološka objašnjenja'!A1" display="METODOLOŠKA OBJAŠNJENJA"/>
     <hyperlink ref="C14" location="'Metodološka objašnjenja'!A1" display="NOTES OF METHODOLOGY"/>
+    <hyperlink ref="A9" location="'7.4.2.'!A1" display="Tab. 7.4.2."/>
+    <hyperlink ref="A11" location="'7.4.3.'!A1" display="Tab. 7.4.3."/>
+    <hyperlink ref="A7" location="'7.4.1.'!A1" display="Tab. 7.4.1."/>
   </hyperlinks>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -3175,21 +3175,21 @@
   <dimension ref="A1:V160"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="7" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="7" topLeftCell="C14" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="31.44140625" customWidth="1"/>
-    <col min="3" max="19" width="7.6640625" customWidth="1"/>
+    <col min="1" max="2" width="31.42578125" customWidth="1"/>
+    <col min="3" max="19" width="7.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="21" t="s">
-        <v>173</v>
+        <v>178</v>
       </c>
       <c r="B1" s="11"/>
       <c r="C1" s="6"/>
@@ -3197,7 +3197,7 @@
       <c r="E1" s="6"/>
       <c r="F1" s="6"/>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>113</v>
       </c>
@@ -3207,7 +3207,7 @@
       <c r="E2" s="3"/>
       <c r="F2" s="3"/>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="7" t="s">
         <v>114</v>
       </c>
@@ -3217,7 +3217,7 @@
       <c r="E3" s="6"/>
       <c r="F3" s="6"/>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>0</v>
       </c>
@@ -3227,7 +3227,7 @@
       <c r="E4" s="6"/>
       <c r="F4" s="6"/>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:22" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="10" t="s">
         <v>1</v>
       </c>
@@ -3237,7 +3237,7 @@
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
     </row>
-    <row r="6" spans="1:22" s="23" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:22" s="23" customFormat="1" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="25"/>
       <c r="B6" s="24"/>
       <c r="C6" s="144" t="s">
@@ -3261,7 +3261,7 @@
       <c r="S6" s="145"/>
       <c r="T6" s="145"/>
     </row>
-    <row r="7" spans="1:22" s="23" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" s="23" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="126" t="s">
         <v>51</v>
       </c>
@@ -3320,7 +3320,7 @@
         <v>95</v>
       </c>
       <c r="T7" s="136" t="s">
-        <v>179</v>
+        <v>173</v>
       </c>
     </row>
     <row r="8" spans="1:22" s="23" customFormat="1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
@@ -3349,7 +3349,7 @@
       <c r="S8" s="116"/>
       <c r="T8" s="116"/>
     </row>
-    <row r="9" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="109" t="s">
         <v>117</v>
       </c>
@@ -3686,7 +3686,7 @@
       <c r="S14" s="143"/>
       <c r="T14" s="143"/>
     </row>
-    <row r="15" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="26" t="s">
         <v>123</v>
       </c>
@@ -3712,7 +3712,7 @@
       <c r="S15" s="121"/>
       <c r="T15" s="121"/>
     </row>
-    <row r="16" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:22" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="109" t="s">
         <v>117</v>
       </c>
@@ -4070,7 +4070,7 @@
       <c r="S22" s="121"/>
       <c r="T22" s="121"/>
     </row>
-    <row r="23" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="109" t="s">
         <v>117</v>
       </c>
@@ -4402,7 +4402,7 @@
       <c r="S28" s="143"/>
       <c r="T28" s="143"/>
     </row>
-    <row r="29" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="26" t="s">
         <v>125</v>
       </c>
@@ -4428,7 +4428,7 @@
       <c r="S29" s="121"/>
       <c r="T29" s="121"/>
     </row>
-    <row r="30" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="109" t="s">
         <v>117</v>
       </c>
@@ -4760,7 +4760,7 @@
       <c r="S35" s="143"/>
       <c r="T35" s="143"/>
     </row>
-    <row r="36" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="26" t="s">
         <v>126</v>
       </c>
@@ -4786,7 +4786,7 @@
       <c r="S36" s="121"/>
       <c r="T36" s="121"/>
     </row>
-    <row r="37" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="109" t="s">
         <v>117</v>
       </c>
@@ -5118,7 +5118,7 @@
       <c r="S42" s="143"/>
       <c r="T42" s="143"/>
     </row>
-    <row r="43" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="26" t="s">
         <v>127</v>
       </c>
@@ -5144,7 +5144,7 @@
       <c r="S43" s="121"/>
       <c r="T43" s="120"/>
     </row>
-    <row r="44" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="109" t="s">
         <v>117</v>
       </c>
@@ -5476,7 +5476,7 @@
       <c r="S49" s="143"/>
       <c r="T49" s="143"/>
     </row>
-    <row r="50" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="26" t="s">
         <v>128</v>
       </c>
@@ -5502,7 +5502,7 @@
       <c r="S50" s="111"/>
       <c r="T50" s="111"/>
     </row>
-    <row r="51" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="109" t="s">
         <v>117</v>
       </c>
@@ -5860,7 +5860,7 @@
       <c r="S57" s="121"/>
       <c r="T57" s="121"/>
     </row>
-    <row r="58" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="109" t="s">
         <v>117</v>
       </c>
@@ -6218,7 +6218,7 @@
       <c r="S64" s="121"/>
       <c r="T64" s="121"/>
     </row>
-    <row r="65" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="109" t="s">
         <v>117</v>
       </c>
@@ -6550,7 +6550,7 @@
       <c r="S70" s="143"/>
       <c r="T70" s="143"/>
     </row>
-    <row r="71" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="26" t="s">
         <v>131</v>
       </c>
@@ -6576,7 +6576,7 @@
       <c r="S71" s="124"/>
       <c r="T71" s="124"/>
     </row>
-    <row r="72" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72" s="109" t="s">
         <v>117</v>
       </c>
@@ -6908,7 +6908,7 @@
       <c r="S77" s="143"/>
       <c r="T77" s="143"/>
     </row>
-    <row r="78" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A78" s="26" t="s">
         <v>132</v>
       </c>
@@ -6934,7 +6934,7 @@
       <c r="S78" s="121"/>
       <c r="T78" s="121"/>
     </row>
-    <row r="79" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A79" s="109" t="s">
         <v>117</v>
       </c>
@@ -7266,7 +7266,7 @@
       <c r="S84" s="143"/>
       <c r="T84" s="143"/>
     </row>
-    <row r="85" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A85" s="26" t="s">
         <v>133</v>
       </c>
@@ -7292,7 +7292,7 @@
       <c r="S85" s="121"/>
       <c r="T85" s="121"/>
     </row>
-    <row r="86" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A86" s="109" t="s">
         <v>117</v>
       </c>
@@ -7650,7 +7650,7 @@
       <c r="S92" s="121"/>
       <c r="T92" s="121"/>
     </row>
-    <row r="93" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93" s="109" t="s">
         <v>117</v>
       </c>
@@ -8008,7 +8008,7 @@
       <c r="S99" s="121"/>
       <c r="T99" s="121"/>
     </row>
-    <row r="100" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100" s="109" t="s">
         <v>117</v>
       </c>
@@ -8340,7 +8340,7 @@
       <c r="S105" s="143"/>
       <c r="T105" s="143"/>
     </row>
-    <row r="106" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A106" s="26" t="s">
         <v>136</v>
       </c>
@@ -8366,7 +8366,7 @@
       <c r="S106" s="121"/>
       <c r="T106" s="121"/>
     </row>
-    <row r="107" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A107" s="109" t="s">
         <v>117</v>
       </c>
@@ -8698,7 +8698,7 @@
       <c r="S112" s="143"/>
       <c r="T112" s="143"/>
     </row>
-    <row r="113" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A113" s="26" t="s">
         <v>137</v>
       </c>
@@ -8724,7 +8724,7 @@
       <c r="S113" s="121"/>
       <c r="T113" s="121"/>
     </row>
-    <row r="114" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A114" s="109" t="s">
         <v>117</v>
       </c>
@@ -9082,7 +9082,7 @@
       <c r="S120" s="121"/>
       <c r="T120" s="121"/>
     </row>
-    <row r="121" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A121" s="109" t="s">
         <v>117</v>
       </c>
@@ -9440,7 +9440,7 @@
       <c r="S127" s="121"/>
       <c r="T127" s="121"/>
     </row>
-    <row r="128" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A128" s="109" t="s">
         <v>117</v>
       </c>
@@ -9798,7 +9798,7 @@
       <c r="S134" s="121"/>
       <c r="T134" s="121"/>
     </row>
-    <row r="135" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A135" s="109" t="s">
         <v>117</v>
       </c>
@@ -10130,7 +10130,7 @@
       <c r="S140" s="143"/>
       <c r="T140" s="143"/>
     </row>
-    <row r="141" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A141" s="26" t="s">
         <v>141</v>
       </c>
@@ -10156,7 +10156,7 @@
       <c r="S141" s="121"/>
       <c r="T141" s="121"/>
     </row>
-    <row r="142" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="109" t="s">
         <v>117</v>
       </c>
@@ -10488,7 +10488,7 @@
       <c r="S147" s="143"/>
       <c r="T147" s="143"/>
     </row>
-    <row r="148" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A148" s="26" t="s">
         <v>142</v>
       </c>
@@ -10514,7 +10514,7 @@
       <c r="S148" s="121"/>
       <c r="T148" s="121"/>
     </row>
-    <row r="149" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A149" s="109" t="s">
         <v>117</v>
       </c>
@@ -10872,7 +10872,7 @@
       <c r="S155" s="121"/>
       <c r="T155" s="121"/>
     </row>
-    <row r="156" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:20" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A156" s="109" t="s">
         <v>117</v>
       </c>
@@ -11231,18 +11231,18 @@
       <pane xSplit="2" ySplit="7" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="31.44140625" customWidth="1"/>
-    <col min="3" max="19" width="7.6640625" customWidth="1"/>
+    <col min="1" max="2" width="31.42578125" customWidth="1"/>
+    <col min="3" max="19" width="7.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
-        <v>174</v>
+        <v>179</v>
       </c>
       <c r="B1" s="14"/>
       <c r="C1" s="17"/>
@@ -11250,7 +11250,7 @@
       <c r="E1" s="17"/>
       <c r="F1" s="17"/>
     </row>
-    <row r="2" spans="1:20" ht="16.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A2" s="13" t="s">
         <v>143</v>
       </c>
@@ -11260,7 +11260,7 @@
       <c r="E2" s="17"/>
       <c r="F2" s="17"/>
     </row>
-    <row r="3" spans="1:20" ht="16.95" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" ht="16.899999999999999" x14ac:dyDescent="0.3">
       <c r="A3" s="88" t="s">
         <v>144</v>
       </c>
@@ -11270,7 +11270,7 @@
       <c r="E3" s="17"/>
       <c r="F3" s="17"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>0</v>
       </c>
@@ -11280,7 +11280,7 @@
       <c r="E4" s="17"/>
       <c r="F4" s="17"/>
     </row>
-    <row r="5" spans="1:20" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
         <v>1</v>
       </c>
@@ -11290,31 +11290,31 @@
       <c r="E5" s="17"/>
       <c r="F5" s="17"/>
     </row>
-    <row r="6" spans="1:20" ht="45.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:20" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="25"/>
       <c r="B6" s="24"/>
-      <c r="C6" s="148" t="s">
+      <c r="C6" s="150" t="s">
         <v>43</v>
       </c>
-      <c r="D6" s="149"/>
-      <c r="E6" s="149"/>
-      <c r="F6" s="149"/>
-      <c r="G6" s="149"/>
-      <c r="H6" s="149"/>
-      <c r="I6" s="149"/>
-      <c r="J6" s="149"/>
-      <c r="K6" s="149"/>
-      <c r="L6" s="149"/>
-      <c r="M6" s="149"/>
-      <c r="N6" s="149"/>
-      <c r="O6" s="149"/>
-      <c r="P6" s="149"/>
-      <c r="Q6" s="149"/>
-      <c r="R6" s="149"/>
-      <c r="S6" s="149"/>
-      <c r="T6" s="149"/>
-    </row>
-    <row r="7" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="D6" s="151"/>
+      <c r="E6" s="151"/>
+      <c r="F6" s="151"/>
+      <c r="G6" s="151"/>
+      <c r="H6" s="151"/>
+      <c r="I6" s="151"/>
+      <c r="J6" s="151"/>
+      <c r="K6" s="151"/>
+      <c r="L6" s="151"/>
+      <c r="M6" s="151"/>
+      <c r="N6" s="151"/>
+      <c r="O6" s="151"/>
+      <c r="P6" s="151"/>
+      <c r="Q6" s="151"/>
+      <c r="R6" s="151"/>
+      <c r="S6" s="151"/>
+      <c r="T6" s="151"/>
+    </row>
+    <row r="7" spans="1:20" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="89" t="s">
         <v>51</v>
       </c>
@@ -11373,10 +11373,10 @@
         <v>95</v>
       </c>
       <c r="T7" s="33" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="8" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="35" t="s">
         <v>19</v>
       </c>
@@ -11402,7 +11402,7 @@
       <c r="S8" s="66"/>
       <c r="T8" s="142"/>
     </row>
-    <row r="9" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="37" t="s">
         <v>44</v>
       </c>
@@ -11464,7 +11464,7 @@
         <v>-17945</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="39" t="s">
         <v>45</v>
       </c>
@@ -11490,7 +11490,7 @@
       <c r="S10" s="65"/>
       <c r="T10" s="67"/>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="41" t="s">
         <v>46</v>
       </c>
@@ -11555,7 +11555,7 @@
         <v>33418</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="41" t="s">
         <v>47</v>
       </c>
@@ -11617,7 +11617,7 @@
         <v>11706</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="39" t="s">
         <v>48</v>
       </c>
@@ -11643,7 +11643,7 @@
       <c r="S13" s="66"/>
       <c r="T13" s="67"/>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="41" t="s">
         <v>49</v>
       </c>
@@ -11707,7 +11707,7 @@
         <v>33418</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="41" t="s">
         <v>50</v>
       </c>
@@ -11769,29 +11769,29 @@
         <v>29651</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="44"/>
       <c r="B16" s="44"/>
-      <c r="C16" s="150"/>
-      <c r="D16" s="151"/>
-      <c r="E16" s="151"/>
-      <c r="F16" s="151"/>
-      <c r="G16" s="151"/>
-      <c r="H16" s="151"/>
-      <c r="I16" s="151"/>
-      <c r="J16" s="151"/>
-      <c r="K16" s="151"/>
-      <c r="L16" s="151"/>
-      <c r="M16" s="151"/>
-      <c r="N16" s="151"/>
-      <c r="O16" s="151"/>
-      <c r="P16" s="151"/>
-      <c r="Q16" s="151"/>
-      <c r="R16" s="151"/>
-      <c r="S16" s="151"/>
-      <c r="T16" s="151"/>
-    </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="C16" s="152"/>
+      <c r="D16" s="153"/>
+      <c r="E16" s="153"/>
+      <c r="F16" s="153"/>
+      <c r="G16" s="153"/>
+      <c r="H16" s="153"/>
+      <c r="I16" s="153"/>
+      <c r="J16" s="153"/>
+      <c r="K16" s="153"/>
+      <c r="L16" s="153"/>
+      <c r="M16" s="153"/>
+      <c r="N16" s="153"/>
+      <c r="O16" s="153"/>
+      <c r="P16" s="153"/>
+      <c r="Q16" s="153"/>
+      <c r="R16" s="153"/>
+      <c r="S16" s="153"/>
+      <c r="T16" s="153"/>
+    </row>
+    <row r="17" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A17" s="43" t="s">
         <v>60</v>
       </c>
@@ -11817,7 +11817,7 @@
       <c r="S17" s="66"/>
       <c r="T17" s="142"/>
     </row>
-    <row r="18" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="37" t="s">
         <v>148</v>
       </c>
@@ -11879,7 +11879,7 @@
         <v>-1366</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="39" t="s">
         <v>45</v>
       </c>
@@ -11943,7 +11943,7 @@
         <v>4354</v>
       </c>
     </row>
-    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A20" s="41" t="s">
         <v>46</v>
       </c>
@@ -12005,7 +12005,7 @@
         <v>3702</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="41" t="s">
         <v>47</v>
       </c>
@@ -12067,7 +12067,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="39" t="s">
         <v>48</v>
       </c>
@@ -12131,7 +12131,7 @@
         <v>5720</v>
       </c>
     </row>
-    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A23" s="41" t="s">
         <v>49</v>
       </c>
@@ -12193,7 +12193,7 @@
         <v>3444</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="41" t="s">
         <v>50</v>
       </c>
@@ -12255,7 +12255,7 @@
         <v>2276</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="44"/>
       <c r="B25" s="44"/>
       <c r="C25" s="146"/>
@@ -12277,7 +12277,7 @@
       <c r="S25" s="147"/>
       <c r="T25" s="147"/>
     </row>
-    <row r="26" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="43" t="s">
         <v>62</v>
       </c>
@@ -12303,7 +12303,7 @@
       <c r="S26" s="66"/>
       <c r="T26" s="142"/>
     </row>
-    <row r="27" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="37" t="s">
         <v>148</v>
       </c>
@@ -12365,7 +12365,7 @@
         <v>-271</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="39" t="s">
         <v>45</v>
       </c>
@@ -12429,7 +12429,7 @@
         <v>954</v>
       </c>
     </row>
-    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A29" s="41" t="s">
         <v>46</v>
       </c>
@@ -12491,7 +12491,7 @@
         <v>836</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A30" s="41" t="s">
         <v>47</v>
       </c>
@@ -12553,7 +12553,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A31" s="39" t="s">
         <v>48</v>
       </c>
@@ -12617,7 +12617,7 @@
         <v>1225</v>
       </c>
     </row>
-    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A32" s="41" t="s">
         <v>49</v>
       </c>
@@ -12679,7 +12679,7 @@
         <v>816</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A33" s="41" t="s">
         <v>50</v>
       </c>
@@ -12741,7 +12741,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="44"/>
       <c r="B34" s="44"/>
       <c r="C34" s="146"/>
@@ -12763,7 +12763,7 @@
       <c r="S34" s="147"/>
       <c r="T34" s="147"/>
     </row>
-    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A35" s="43" t="s">
         <v>63</v>
       </c>
@@ -12789,7 +12789,7 @@
       <c r="S35" s="66"/>
       <c r="T35" s="142"/>
     </row>
-    <row r="36" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A36" s="37" t="s">
         <v>148</v>
       </c>
@@ -12851,7 +12851,7 @@
         <v>-2186</v>
       </c>
     </row>
-    <row r="37" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A37" s="39" t="s">
         <v>45</v>
       </c>
@@ -12915,7 +12915,7 @@
         <v>1172</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A38" s="41" t="s">
         <v>46</v>
       </c>
@@ -12977,7 +12977,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A39" s="41" t="s">
         <v>47</v>
       </c>
@@ -13039,7 +13039,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="40" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A40" s="39" t="s">
         <v>48</v>
       </c>
@@ -13103,7 +13103,7 @@
         <v>3358</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A41" s="41" t="s">
         <v>49</v>
       </c>
@@ -13165,7 +13165,7 @@
         <v>1610</v>
       </c>
     </row>
-    <row r="42" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A42" s="41" t="s">
         <v>50</v>
       </c>
@@ -13227,7 +13227,7 @@
         <v>1748</v>
       </c>
     </row>
-    <row r="43" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="44"/>
       <c r="B43" s="44"/>
       <c r="C43" s="146"/>
@@ -13249,7 +13249,7 @@
       <c r="S43" s="147"/>
       <c r="T43" s="147"/>
     </row>
-    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A44" s="43" t="s">
         <v>64</v>
       </c>
@@ -13275,7 +13275,7 @@
       <c r="S44" s="66"/>
       <c r="T44" s="142"/>
     </row>
-    <row r="45" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A45" s="37" t="s">
         <v>148</v>
       </c>
@@ -13337,7 +13337,7 @@
         <v>-664</v>
       </c>
     </row>
-    <row r="46" spans="1:20" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:20" ht="14.45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A46" s="39" t="s">
         <v>45</v>
       </c>
@@ -13401,7 +13401,7 @@
         <v>1171</v>
       </c>
     </row>
-    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A47" s="41" t="s">
         <v>46</v>
       </c>
@@ -13463,7 +13463,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:20" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A48" s="41" t="s">
         <v>47</v>
       </c>
@@ -13525,7 +13525,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:20" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A49" s="39" t="s">
         <v>48</v>
       </c>
@@ -13589,7 +13589,7 @@
         <v>1835</v>
       </c>
     </row>
-    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A50" s="41" t="s">
         <v>49</v>
       </c>
@@ -13651,7 +13651,7 @@
         <v>934</v>
       </c>
     </row>
-    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A51" s="41" t="s">
         <v>50</v>
       </c>
@@ -13713,7 +13713,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="52" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A52" s="45"/>
       <c r="B52" s="44"/>
       <c r="C52" s="146"/>
@@ -13735,7 +13735,7 @@
       <c r="S52" s="147"/>
       <c r="T52" s="147"/>
     </row>
-    <row r="53" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A53" s="43" t="s">
         <v>65</v>
       </c>
@@ -13761,7 +13761,7 @@
       <c r="S53" s="66"/>
       <c r="T53" s="142"/>
     </row>
-    <row r="54" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A54" s="37" t="s">
         <v>148</v>
       </c>
@@ -13823,7 +13823,7 @@
         <v>-544</v>
       </c>
     </row>
-    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A55" s="39" t="s">
         <v>45</v>
       </c>
@@ -13887,7 +13887,7 @@
         <v>1121</v>
       </c>
     </row>
-    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A56" s="41" t="s">
         <v>46</v>
       </c>
@@ -13949,7 +13949,7 @@
         <v>918</v>
       </c>
     </row>
-    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A57" s="41" t="s">
         <v>47</v>
       </c>
@@ -14011,7 +14011,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A58" s="39" t="s">
         <v>48</v>
       </c>
@@ -14075,7 +14075,7 @@
         <v>1665</v>
       </c>
     </row>
-    <row r="59" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A59" s="41" t="s">
         <v>49</v>
       </c>
@@ -14137,7 +14137,7 @@
         <v>865</v>
       </c>
     </row>
-    <row r="60" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A60" s="41" t="s">
         <v>50</v>
       </c>
@@ -14199,7 +14199,7 @@
         <v>800</v>
       </c>
     </row>
-    <row r="61" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A61" s="44"/>
       <c r="B61" s="44"/>
       <c r="C61" s="146"/>
@@ -14221,7 +14221,7 @@
       <c r="S61" s="147"/>
       <c r="T61" s="147"/>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A62" s="43" t="s">
         <v>67</v>
       </c>
@@ -14247,7 +14247,7 @@
       <c r="S62" s="66"/>
       <c r="T62" s="142"/>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A63" s="37" t="s">
         <v>148</v>
       </c>
@@ -14309,7 +14309,7 @@
         <v>-621</v>
       </c>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A64" s="39" t="s">
         <v>45</v>
       </c>
@@ -14373,7 +14373,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65" s="41" t="s">
         <v>46</v>
       </c>
@@ -14435,7 +14435,7 @@
         <v>523</v>
       </c>
     </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66" s="41" t="s">
         <v>47</v>
       </c>
@@ -14497,7 +14497,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67" s="39" t="s">
         <v>48</v>
       </c>
@@ -14561,7 +14561,7 @@
         <v>1234</v>
       </c>
     </row>
-    <row r="68" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A68" s="41" t="s">
         <v>49</v>
       </c>
@@ -14623,7 +14623,7 @@
         <v>860</v>
       </c>
     </row>
-    <row r="69" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A69" s="41" t="s">
         <v>50</v>
       </c>
@@ -14685,7 +14685,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="70" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A70" s="44"/>
       <c r="B70" s="44"/>
       <c r="C70" s="146"/>
@@ -14707,7 +14707,7 @@
       <c r="S70" s="147"/>
       <c r="T70" s="147"/>
     </row>
-    <row r="71" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A71" s="43" t="s">
         <v>68</v>
       </c>
@@ -14733,7 +14733,7 @@
       <c r="S71" s="66"/>
       <c r="T71" s="142"/>
     </row>
-    <row r="72" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A72" s="37" t="s">
         <v>148</v>
       </c>
@@ -14795,7 +14795,7 @@
         <v>-1115</v>
       </c>
     </row>
-    <row r="73" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A73" s="39" t="s">
         <v>45</v>
       </c>
@@ -14859,7 +14859,7 @@
         <v>752</v>
       </c>
     </row>
-    <row r="74" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A74" s="41" t="s">
         <v>46</v>
       </c>
@@ -14921,7 +14921,7 @@
         <v>635</v>
       </c>
     </row>
-    <row r="75" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A75" s="41" t="s">
         <v>47</v>
       </c>
@@ -14983,7 +14983,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="76" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A76" s="39" t="s">
         <v>48</v>
       </c>
@@ -15047,7 +15047,7 @@
         <v>1867</v>
       </c>
     </row>
-    <row r="77" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A77" s="41" t="s">
         <v>49</v>
       </c>
@@ -15109,7 +15109,7 @@
         <v>1246</v>
       </c>
     </row>
-    <row r="78" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A78" s="41" t="s">
         <v>50</v>
       </c>
@@ -15171,7 +15171,7 @@
         <v>621</v>
       </c>
     </row>
-    <row r="79" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A79" s="44"/>
       <c r="B79" s="44"/>
       <c r="C79" s="146"/>
@@ -15193,7 +15193,7 @@
       <c r="S79" s="147"/>
       <c r="T79" s="147"/>
     </row>
-    <row r="80" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A80" s="43" t="s">
         <v>69</v>
       </c>
@@ -15219,7 +15219,7 @@
       <c r="S80" s="66"/>
       <c r="T80" s="142"/>
     </row>
-    <row r="81" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A81" s="37" t="s">
         <v>148</v>
       </c>
@@ -15281,7 +15281,7 @@
         <v>-1153</v>
       </c>
     </row>
-    <row r="82" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A82" s="39" t="s">
         <v>45</v>
       </c>
@@ -15345,7 +15345,7 @@
         <v>3404</v>
       </c>
     </row>
-    <row r="83" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A83" s="41" t="s">
         <v>46</v>
       </c>
@@ -15407,7 +15407,7 @@
         <v>2355</v>
       </c>
     </row>
-    <row r="84" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A84" s="41" t="s">
         <v>47</v>
       </c>
@@ -15469,7 +15469,7 @@
         <v>1049</v>
       </c>
     </row>
-    <row r="85" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A85" s="39" t="s">
         <v>48</v>
       </c>
@@ -15533,7 +15533,7 @@
         <v>4557</v>
       </c>
     </row>
-    <row r="86" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A86" s="41" t="s">
         <v>49</v>
       </c>
@@ -15595,7 +15595,7 @@
         <v>2008</v>
       </c>
     </row>
-    <row r="87" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A87" s="41" t="s">
         <v>50</v>
       </c>
@@ -15657,7 +15657,7 @@
         <v>2549</v>
       </c>
     </row>
-    <row r="88" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A88" s="44"/>
       <c r="B88" s="44"/>
       <c r="C88" s="146"/>
@@ -15679,7 +15679,7 @@
       <c r="S88" s="147"/>
       <c r="T88" s="147"/>
     </row>
-    <row r="89" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A89" s="43" t="s">
         <v>70</v>
       </c>
@@ -15705,7 +15705,7 @@
       <c r="S89" s="66"/>
       <c r="T89" s="142"/>
     </row>
-    <row r="90" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A90" s="37" t="s">
         <v>148</v>
       </c>
@@ -15767,7 +15767,7 @@
         <v>-404</v>
       </c>
     </row>
-    <row r="91" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A91" s="39" t="s">
         <v>45</v>
       </c>
@@ -15831,7 +15831,7 @@
         <v>664</v>
       </c>
     </row>
-    <row r="92" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A92" s="41" t="s">
         <v>46</v>
       </c>
@@ -15893,7 +15893,7 @@
         <v>517</v>
       </c>
     </row>
-    <row r="93" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A93" s="41" t="s">
         <v>47</v>
       </c>
@@ -15955,7 +15955,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="94" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A94" s="39" t="s">
         <v>48</v>
       </c>
@@ -16019,7 +16019,7 @@
         <v>1068</v>
       </c>
     </row>
-    <row r="95" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A95" s="41" t="s">
         <v>49</v>
       </c>
@@ -16081,7 +16081,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="96" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A96" s="41" t="s">
         <v>50</v>
       </c>
@@ -16143,7 +16143,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="97" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A97" s="45"/>
       <c r="B97" s="44"/>
       <c r="C97" s="146"/>
@@ -16165,7 +16165,7 @@
       <c r="S97" s="147"/>
       <c r="T97" s="147"/>
     </row>
-    <row r="98" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A98" s="43" t="s">
         <v>71</v>
       </c>
@@ -16191,7 +16191,7 @@
       <c r="S98" s="66"/>
       <c r="T98" s="142"/>
     </row>
-    <row r="99" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A99" s="37" t="s">
         <v>148</v>
       </c>
@@ -16253,7 +16253,7 @@
         <v>-1172</v>
       </c>
     </row>
-    <row r="100" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A100" s="39" t="s">
         <v>45</v>
       </c>
@@ -16317,7 +16317,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="101" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A101" s="41" t="s">
         <v>46</v>
       </c>
@@ -16379,7 +16379,7 @@
         <v>428</v>
       </c>
     </row>
-    <row r="102" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A102" s="41" t="s">
         <v>47</v>
       </c>
@@ -16441,7 +16441,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="103" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A103" s="39" t="s">
         <v>48</v>
       </c>
@@ -16505,7 +16505,7 @@
         <v>1699</v>
       </c>
     </row>
-    <row r="104" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A104" s="41" t="s">
         <v>49</v>
       </c>
@@ -16567,7 +16567,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="105" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A105" s="41" t="s">
         <v>50</v>
       </c>
@@ -16629,7 +16629,7 @@
         <v>804</v>
       </c>
     </row>
-    <row r="106" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A106" s="44"/>
       <c r="B106" s="44"/>
       <c r="C106" s="146"/>
@@ -16651,7 +16651,7 @@
       <c r="S106" s="147"/>
       <c r="T106" s="147"/>
     </row>
-    <row r="107" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A107" s="43" t="s">
         <v>72</v>
       </c>
@@ -16677,7 +16677,7 @@
       <c r="S107" s="66"/>
       <c r="T107" s="142"/>
     </row>
-    <row r="108" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A108" s="37" t="s">
         <v>148</v>
       </c>
@@ -16739,7 +16739,7 @@
         <v>-1243</v>
       </c>
     </row>
-    <row r="109" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A109" s="39" t="s">
         <v>45</v>
       </c>
@@ -16803,7 +16803,7 @@
         <v>689</v>
       </c>
     </row>
-    <row r="110" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A110" s="41" t="s">
         <v>46</v>
       </c>
@@ -16865,7 +16865,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="111" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A111" s="41" t="s">
         <v>47</v>
       </c>
@@ -16927,7 +16927,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="112" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A112" s="39" t="s">
         <v>48</v>
       </c>
@@ -16991,7 +16991,7 @@
         <v>1932</v>
       </c>
     </row>
-    <row r="113" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A113" s="41" t="s">
         <v>49</v>
       </c>
@@ -17053,7 +17053,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="114" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A114" s="41" t="s">
         <v>50</v>
       </c>
@@ -17115,7 +17115,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="115" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A115" s="44"/>
       <c r="B115" s="44"/>
       <c r="C115" s="146"/>
@@ -17137,7 +17137,7 @@
       <c r="S115" s="147"/>
       <c r="T115" s="147"/>
     </row>
-    <row r="116" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A116" s="43" t="s">
         <v>73</v>
       </c>
@@ -17163,7 +17163,7 @@
       <c r="S116" s="66"/>
       <c r="T116" s="142"/>
     </row>
-    <row r="117" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A117" s="37" t="s">
         <v>148</v>
       </c>
@@ -17225,7 +17225,7 @@
         <v>-2254</v>
       </c>
     </row>
-    <row r="118" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A118" s="39" t="s">
         <v>45</v>
       </c>
@@ -17289,7 +17289,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="119" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A119" s="41" t="s">
         <v>46</v>
       </c>
@@ -17351,7 +17351,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="120" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A120" s="41" t="s">
         <v>47</v>
       </c>
@@ -17413,7 +17413,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="121" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A121" s="39" t="s">
         <v>48</v>
       </c>
@@ -17477,7 +17477,7 @@
         <v>3173</v>
       </c>
     </row>
-    <row r="122" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A122" s="41" t="s">
         <v>49</v>
       </c>
@@ -17539,7 +17539,7 @@
         <v>1602</v>
       </c>
     </row>
-    <row r="123" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A123" s="41" t="s">
         <v>50</v>
       </c>
@@ -17601,7 +17601,7 @@
         <v>1571</v>
       </c>
     </row>
-    <row r="124" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A124" s="44"/>
       <c r="B124" s="44"/>
       <c r="C124" s="146"/>
@@ -17623,7 +17623,7 @@
       <c r="S124" s="147"/>
       <c r="T124" s="147"/>
     </row>
-    <row r="125" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A125" s="43" t="s">
         <v>74</v>
       </c>
@@ -17649,7 +17649,7 @@
       <c r="S125" s="66"/>
       <c r="T125" s="142"/>
     </row>
-    <row r="126" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A126" s="37" t="s">
         <v>148</v>
       </c>
@@ -17711,7 +17711,7 @@
         <v>-618</v>
       </c>
     </row>
-    <row r="127" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A127" s="39" t="s">
         <v>45</v>
       </c>
@@ -17775,7 +17775,7 @@
         <v>2183</v>
       </c>
     </row>
-    <row r="128" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A128" s="41" t="s">
         <v>46</v>
       </c>
@@ -17837,7 +17837,7 @@
         <v>1571</v>
       </c>
     </row>
-    <row r="129" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A129" s="41" t="s">
         <v>47</v>
       </c>
@@ -17899,7 +17899,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="130" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A130" s="39" t="s">
         <v>48</v>
       </c>
@@ -17963,7 +17963,7 @@
         <v>2801</v>
       </c>
     </row>
-    <row r="131" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A131" s="41" t="s">
         <v>49</v>
       </c>
@@ -18025,7 +18025,7 @@
         <v>1259</v>
       </c>
     </row>
-    <row r="132" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A132" s="41" t="s">
         <v>50</v>
       </c>
@@ -18087,7 +18087,7 @@
         <v>1542</v>
       </c>
     </row>
-    <row r="133" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A133" s="46"/>
       <c r="B133" s="46"/>
       <c r="C133" s="146"/>
@@ -18109,7 +18109,7 @@
       <c r="S133" s="147"/>
       <c r="T133" s="147"/>
     </row>
-    <row r="134" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A134" s="35" t="s">
         <v>76</v>
       </c>
@@ -18135,7 +18135,7 @@
       <c r="S134" s="66"/>
       <c r="T134" s="142"/>
     </row>
-    <row r="135" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A135" s="37" t="s">
         <v>148</v>
       </c>
@@ -18197,7 +18197,7 @@
         <v>-2634</v>
       </c>
     </row>
-    <row r="136" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A136" s="39" t="s">
         <v>45</v>
       </c>
@@ -18261,7 +18261,7 @@
         <v>1824</v>
       </c>
     </row>
-    <row r="137" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A137" s="41" t="s">
         <v>46</v>
       </c>
@@ -18323,7 +18323,7 @@
         <v>1354</v>
       </c>
     </row>
-    <row r="138" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A138" s="41" t="s">
         <v>47</v>
       </c>
@@ -18385,7 +18385,7 @@
         <v>470</v>
       </c>
     </row>
-    <row r="139" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A139" s="39" t="s">
         <v>48</v>
       </c>
@@ -18449,7 +18449,7 @@
         <v>4458</v>
       </c>
     </row>
-    <row r="140" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A140" s="41" t="s">
         <v>49</v>
       </c>
@@ -18511,7 +18511,7 @@
         <v>2246</v>
       </c>
     </row>
-    <row r="141" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A141" s="41" t="s">
         <v>50</v>
       </c>
@@ -18573,7 +18573,7 @@
         <v>2212</v>
       </c>
     </row>
-    <row r="142" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A142" s="46"/>
       <c r="B142" s="46"/>
       <c r="C142" s="146"/>
@@ -18595,7 +18595,7 @@
       <c r="S142" s="147"/>
       <c r="T142" s="147"/>
     </row>
-    <row r="143" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A143" s="35" t="s">
         <v>77</v>
       </c>
@@ -18621,7 +18621,7 @@
       <c r="S143" s="66"/>
       <c r="T143" s="142"/>
     </row>
-    <row r="144" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A144" s="37" t="s">
         <v>148</v>
       </c>
@@ -18683,7 +18683,7 @@
         <v>-658</v>
       </c>
     </row>
-    <row r="145" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A145" s="39" t="s">
         <v>45</v>
       </c>
@@ -18747,7 +18747,7 @@
         <v>1287</v>
       </c>
     </row>
-    <row r="146" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A146" s="41" t="s">
         <v>46</v>
       </c>
@@ -18809,7 +18809,7 @@
         <v>872</v>
       </c>
     </row>
-    <row r="147" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A147" s="41" t="s">
         <v>47</v>
       </c>
@@ -18871,7 +18871,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="148" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A148" s="39" t="s">
         <v>48</v>
       </c>
@@ -18935,7 +18935,7 @@
         <v>1945</v>
       </c>
     </row>
-    <row r="149" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A149" s="41" t="s">
         <v>49</v>
       </c>
@@ -18997,7 +18997,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="150" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A150" s="41" t="s">
         <v>50</v>
       </c>
@@ -19059,7 +19059,7 @@
         <v>929</v>
       </c>
     </row>
-    <row r="151" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A151" s="46"/>
       <c r="B151" s="46"/>
       <c r="C151" s="146"/>
@@ -19081,7 +19081,7 @@
       <c r="S151" s="147"/>
       <c r="T151" s="147"/>
     </row>
-    <row r="152" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A152" s="35" t="s">
         <v>78</v>
       </c>
@@ -19107,7 +19107,7 @@
       <c r="S152" s="66"/>
       <c r="T152" s="142"/>
     </row>
-    <row r="153" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A153" s="37" t="s">
         <v>148</v>
       </c>
@@ -19169,7 +19169,7 @@
         <v>-2712</v>
       </c>
     </row>
-    <row r="154" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A154" s="39" t="s">
         <v>45</v>
       </c>
@@ -19233,7 +19233,7 @@
         <v>1165</v>
       </c>
     </row>
-    <row r="155" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A155" s="41" t="s">
         <v>46</v>
       </c>
@@ -19295,7 +19295,7 @@
         <v>731</v>
       </c>
     </row>
-    <row r="156" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A156" s="41" t="s">
         <v>47</v>
       </c>
@@ -19357,7 +19357,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="157" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A157" s="39" t="s">
         <v>48</v>
       </c>
@@ -19421,7 +19421,7 @@
         <v>3877</v>
       </c>
     </row>
-    <row r="158" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A158" s="41" t="s">
         <v>49</v>
       </c>
@@ -19483,7 +19483,7 @@
         <v>1910</v>
       </c>
     </row>
-    <row r="159" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A159" s="41" t="s">
         <v>50</v>
       </c>
@@ -19545,7 +19545,7 @@
         <v>1967</v>
       </c>
     </row>
-    <row r="160" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A160" s="46"/>
       <c r="B160" s="46"/>
       <c r="C160" s="146"/>
@@ -19567,7 +19567,7 @@
       <c r="S160" s="147"/>
       <c r="T160" s="147"/>
     </row>
-    <row r="161" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A161" s="35" t="s">
         <v>79</v>
       </c>
@@ -19593,7 +19593,7 @@
       <c r="S161" s="66"/>
       <c r="T161" s="142"/>
     </row>
-    <row r="162" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A162" s="37" t="s">
         <v>148</v>
       </c>
@@ -19655,7 +19655,7 @@
         <v>-346</v>
       </c>
     </row>
-    <row r="163" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A163" s="39" t="s">
         <v>45</v>
       </c>
@@ -19719,7 +19719,7 @@
         <v>3983</v>
       </c>
     </row>
-    <row r="164" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A164" s="41" t="s">
         <v>46</v>
       </c>
@@ -19781,7 +19781,7 @@
         <v>2155</v>
       </c>
     </row>
-    <row r="165" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A165" s="41" t="s">
         <v>47</v>
       </c>
@@ -19843,7 +19843,7 @@
         <v>1828</v>
       </c>
     </row>
-    <row r="166" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A166" s="39" t="s">
         <v>48</v>
       </c>
@@ -19907,7 +19907,7 @@
         <v>4329</v>
       </c>
     </row>
-    <row r="167" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A167" s="41" t="s">
         <v>49</v>
       </c>
@@ -19969,7 +19969,7 @@
         <v>2174</v>
       </c>
     </row>
-    <row r="168" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A168" s="41" t="s">
         <v>50</v>
       </c>
@@ -20031,7 +20031,7 @@
         <v>2155</v>
       </c>
     </row>
-    <row r="169" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A169" s="46"/>
       <c r="B169" s="46"/>
       <c r="C169" s="146"/>
@@ -20053,7 +20053,7 @@
       <c r="S169" s="147"/>
       <c r="T169" s="147"/>
     </row>
-    <row r="170" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A170" s="35" t="s">
         <v>80</v>
       </c>
@@ -20079,7 +20079,7 @@
       <c r="S170" s="66"/>
       <c r="T170" s="142"/>
     </row>
-    <row r="171" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A171" s="37" t="s">
         <v>148</v>
       </c>
@@ -20141,7 +20141,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="172" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A172" s="39" t="s">
         <v>45</v>
       </c>
@@ -20205,7 +20205,7 @@
         <v>2800</v>
       </c>
     </row>
-    <row r="173" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A173" s="41" t="s">
         <v>46</v>
       </c>
@@ -20267,7 +20267,7 @@
         <v>1724</v>
       </c>
     </row>
-    <row r="174" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A174" s="41" t="s">
         <v>47</v>
       </c>
@@ -20329,7 +20329,7 @@
         <v>1076</v>
       </c>
     </row>
-    <row r="175" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A175" s="39" t="s">
         <v>48</v>
       </c>
@@ -20393,7 +20393,7 @@
         <v>2410</v>
       </c>
     </row>
-    <row r="176" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A176" s="41" t="s">
         <v>49</v>
       </c>
@@ -20455,7 +20455,7 @@
         <v>1130</v>
       </c>
     </row>
-    <row r="177" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A177" s="41" t="s">
         <v>50</v>
       </c>
@@ -20517,7 +20517,7 @@
         <v>1280</v>
       </c>
     </row>
-    <row r="178" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A178" s="46"/>
       <c r="B178" s="46"/>
       <c r="C178" s="146"/>
@@ -20539,7 +20539,7 @@
       <c r="S178" s="147"/>
       <c r="T178" s="147"/>
     </row>
-    <row r="179" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A179" s="35" t="s">
         <v>81</v>
       </c>
@@ -20565,7 +20565,7 @@
       <c r="S179" s="66"/>
       <c r="T179" s="142"/>
     </row>
-    <row r="180" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A180" s="37" t="s">
         <v>148</v>
       </c>
@@ -20627,7 +20627,7 @@
         <v>-84</v>
       </c>
     </row>
-    <row r="181" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A181" s="39" t="s">
         <v>45</v>
       </c>
@@ -20691,7 +20691,7 @@
         <v>1404</v>
       </c>
     </row>
-    <row r="182" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A182" s="41" t="s">
         <v>46</v>
       </c>
@@ -20753,7 +20753,7 @@
         <v>939</v>
       </c>
     </row>
-    <row r="183" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A183" s="41" t="s">
         <v>47</v>
       </c>
@@ -20815,7 +20815,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="184" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A184" s="39" t="s">
         <v>48</v>
       </c>
@@ -20879,7 +20879,7 @@
         <v>1488</v>
       </c>
     </row>
-    <row r="185" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A185" s="41" t="s">
         <v>49</v>
       </c>
@@ -20941,7 +20941,7 @@
         <v>904</v>
       </c>
     </row>
-    <row r="186" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A186" s="41" t="s">
         <v>50</v>
       </c>
@@ -21003,7 +21003,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="187" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A187" s="46"/>
       <c r="B187" s="46"/>
       <c r="C187" s="146"/>
@@ -21025,7 +21025,7 @@
       <c r="S187" s="147"/>
       <c r="T187" s="147"/>
     </row>
-    <row r="188" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A188" s="35" t="s">
         <v>82</v>
       </c>
@@ -21051,7 +21051,7 @@
       <c r="S188" s="66"/>
       <c r="T188" s="142"/>
     </row>
-    <row r="189" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A189" s="37" t="s">
         <v>148</v>
       </c>
@@ -21113,7 +21113,7 @@
         <v>-422</v>
       </c>
     </row>
-    <row r="190" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A190" s="39" t="s">
         <v>45</v>
       </c>
@@ -21177,7 +21177,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="191" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A191" s="41" t="s">
         <v>46</v>
       </c>
@@ -21239,7 +21239,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="192" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A192" s="41" t="s">
         <v>47</v>
       </c>
@@ -21301,7 +21301,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="193" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A193" s="39" t="s">
         <v>48</v>
       </c>
@@ -21365,7 +21365,7 @@
         <v>916</v>
       </c>
     </row>
-    <row r="194" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A194" s="41" t="s">
         <v>49</v>
       </c>
@@ -21427,7 +21427,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="195" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A195" s="41" t="s">
         <v>50</v>
       </c>
@@ -21489,7 +21489,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="196" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A196" s="46"/>
       <c r="B196" s="46"/>
       <c r="C196" s="146"/>
@@ -21511,7 +21511,7 @@
       <c r="S196" s="147"/>
       <c r="T196" s="147"/>
     </row>
-    <row r="197" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A197" s="35" t="s">
         <v>83</v>
       </c>
@@ -21537,7 +21537,7 @@
       <c r="S197" s="66"/>
       <c r="T197" s="142"/>
     </row>
-    <row r="198" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A198" s="37" t="s">
         <v>148</v>
       </c>
@@ -21599,7 +21599,7 @@
         <v>2132</v>
       </c>
     </row>
-    <row r="199" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A199" s="39" t="s">
         <v>45</v>
       </c>
@@ -21663,7 +21663,7 @@
         <v>13644</v>
       </c>
     </row>
-    <row r="200" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A200" s="41" t="s">
         <v>46</v>
       </c>
@@ -21725,7 +21725,7 @@
         <v>10886</v>
       </c>
     </row>
-    <row r="201" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A201" s="41" t="s">
         <v>47</v>
       </c>
@@ -21787,7 +21787,7 @@
         <v>2758</v>
       </c>
     </row>
-    <row r="202" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A202" s="39" t="s">
         <v>48</v>
       </c>
@@ -21851,7 +21851,7 @@
         <v>11512</v>
       </c>
     </row>
-    <row r="203" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A203" s="41" t="s">
         <v>49</v>
       </c>
@@ -21913,7 +21913,7 @@
         <v>6466</v>
       </c>
     </row>
-    <row r="204" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A204" s="41" t="s">
         <v>50</v>
       </c>
@@ -21975,11 +21975,11 @@
         <v>5046</v>
       </c>
     </row>
-    <row r="206" spans="1:20" ht="41.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A206" s="153" t="s">
+    <row r="206" spans="1:20" ht="41.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A206" s="149" t="s">
         <v>84</v>
       </c>
-      <c r="B206" s="153"/>
+      <c r="B206" s="149"/>
       <c r="C206" s="48"/>
       <c r="D206" s="48"/>
       <c r="E206" s="48"/>
@@ -21990,11 +21990,11 @@
       <c r="J206" s="48"/>
       <c r="K206" s="48"/>
     </row>
-    <row r="208" spans="1:20" ht="48.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A208" s="152" t="s">
+    <row r="208" spans="1:20" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A208" s="148" t="s">
         <v>150</v>
       </c>
-      <c r="B208" s="152"/>
+      <c r="B208" s="148"/>
     </row>
   </sheetData>
   <mergeCells count="24">
@@ -22043,22 +22043,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S71"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="2" ySplit="7" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="31.44140625" customWidth="1"/>
-    <col min="3" max="15" width="9.6640625" customWidth="1"/>
+    <col min="1" max="2" width="31.42578125" customWidth="1"/>
+    <col min="3" max="15" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A1" s="49" t="s">
-        <v>175</v>
+        <v>181</v>
       </c>
       <c r="B1" s="50"/>
       <c r="C1" s="51"/>
@@ -22079,7 +22079,7 @@
       <c r="R1" s="23"/>
       <c r="S1" s="23"/>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A2" s="52" t="s">
         <v>172</v>
       </c>
@@ -22102,7 +22102,7 @@
       <c r="R2" s="23"/>
       <c r="S2" s="23"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A3" s="127" t="s">
         <v>152</v>
       </c>
@@ -22125,7 +22125,7 @@
       <c r="R3" s="23"/>
       <c r="S3" s="23"/>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="57" t="s">
         <v>0</v>
       </c>
@@ -22148,7 +22148,7 @@
       <c r="R4" s="23"/>
       <c r="S4" s="23"/>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A5" s="59" t="s">
         <v>1</v>
       </c>
@@ -22194,7 +22194,7 @@
       <c r="R6" s="23"/>
       <c r="S6" s="23"/>
     </row>
-    <row r="7" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="89" t="s">
         <v>51</v>
       </c>
@@ -22244,12 +22244,12 @@
         <v>157</v>
       </c>
       <c r="Q7" s="34" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="R7" s="23"/>
       <c r="S7" s="23"/>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A8" s="77" t="s">
         <v>19</v>
       </c>
@@ -22304,7 +22304,7 @@
       <c r="R8" s="23"/>
       <c r="S8" s="141"/>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="77" t="s">
         <v>60</v>
       </c>
@@ -22359,7 +22359,7 @@
       <c r="R9" s="23"/>
       <c r="S9" s="23"/>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A10" s="77" t="s">
         <v>62</v>
       </c>
@@ -22414,7 +22414,7 @@
       <c r="R10" s="23"/>
       <c r="S10" s="23"/>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="77" t="s">
         <v>63</v>
       </c>
@@ -22469,7 +22469,7 @@
       <c r="R11" s="23"/>
       <c r="S11" s="23"/>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="77" t="s">
         <v>64</v>
       </c>
@@ -22524,7 +22524,7 @@
       <c r="R12" s="23"/>
       <c r="S12" s="23"/>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="77" t="s">
         <v>65</v>
       </c>
@@ -22579,7 +22579,7 @@
       <c r="R13" s="23"/>
       <c r="S13" s="23"/>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14" s="77" t="s">
         <v>67</v>
       </c>
@@ -22634,7 +22634,7 @@
       <c r="R14" s="23"/>
       <c r="S14" s="23"/>
     </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A15" s="77" t="s">
         <v>68</v>
       </c>
@@ -22689,7 +22689,7 @@
       <c r="R15" s="23"/>
       <c r="S15" s="23"/>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="77" t="s">
         <v>69</v>
       </c>
@@ -22744,7 +22744,7 @@
       <c r="R16" s="23"/>
       <c r="S16" s="23"/>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="77" t="s">
         <v>70</v>
       </c>
@@ -22799,7 +22799,7 @@
       <c r="R17" s="23"/>
       <c r="S17" s="23"/>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="77" t="s">
         <v>71</v>
       </c>
@@ -22854,7 +22854,7 @@
       <c r="R18" s="23"/>
       <c r="S18" s="23"/>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="77" t="s">
         <v>72</v>
       </c>
@@ -22909,7 +22909,7 @@
       <c r="R19" s="23"/>
       <c r="S19" s="23"/>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="77" t="s">
         <v>73</v>
       </c>
@@ -22964,7 +22964,7 @@
       <c r="R20" s="23"/>
       <c r="S20" s="23"/>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A21" s="77" t="s">
         <v>74</v>
       </c>
@@ -23019,7 +23019,7 @@
       <c r="R21" s="23"/>
       <c r="S21" s="23"/>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="77" t="s">
         <v>76</v>
       </c>
@@ -23074,7 +23074,7 @@
       <c r="R22" s="23"/>
       <c r="S22" s="23"/>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="77" t="s">
         <v>77</v>
       </c>
@@ -23129,7 +23129,7 @@
       <c r="R23" s="23"/>
       <c r="S23" s="23"/>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A24" s="77" t="s">
         <v>78</v>
       </c>
@@ -23184,7 +23184,7 @@
       <c r="R24" s="23"/>
       <c r="S24" s="23"/>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A25" s="77" t="s">
         <v>79</v>
       </c>
@@ -23239,7 +23239,7 @@
       <c r="R25" s="23"/>
       <c r="S25" s="23"/>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A26" s="77" t="s">
         <v>80</v>
       </c>
@@ -23294,7 +23294,7 @@
       <c r="R26" s="23"/>
       <c r="S26" s="23"/>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A27" s="77" t="s">
         <v>81</v>
       </c>
@@ -23349,7 +23349,7 @@
       <c r="R27" s="23"/>
       <c r="S27" s="23"/>
     </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A28" s="77" t="s">
         <v>82</v>
       </c>
@@ -23404,7 +23404,7 @@
       <c r="R28" s="23"/>
       <c r="S28" s="23"/>
     </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A29" s="77" t="s">
         <v>83</v>
       </c>
@@ -23459,7 +23459,7 @@
       <c r="R29" s="23"/>
       <c r="S29" s="23"/>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A30" s="23"/>
       <c r="B30" s="23"/>
       <c r="C30" s="23"/>
@@ -23480,7 +23480,7 @@
       <c r="R30" s="23"/>
       <c r="S30" s="23"/>
     </row>
-    <row r="31" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:19" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="155" t="s">
         <v>158</v>
       </c>
@@ -23503,7 +23503,7 @@
       <c r="R31" s="23"/>
       <c r="S31" s="23"/>
     </row>
-    <row r="32" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:19" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="156" t="s">
         <v>159</v>
       </c>
@@ -23526,7 +23526,7 @@
       <c r="R32" s="23"/>
       <c r="S32" s="23"/>
     </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A33" s="131"/>
       <c r="B33" s="131"/>
       <c r="C33" s="23"/>
@@ -23593,7 +23593,7 @@
       <c r="R35" s="23"/>
       <c r="S35" s="23"/>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A36" s="23"/>
       <c r="B36" s="23"/>
       <c r="C36" s="23"/>
@@ -23614,7 +23614,7 @@
       <c r="R36" s="23"/>
       <c r="S36" s="23"/>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A37" s="23"/>
       <c r="B37" s="23"/>
       <c r="C37" s="23"/>
@@ -23635,7 +23635,7 @@
       <c r="R37" s="23"/>
       <c r="S37" s="23"/>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A38" s="23"/>
       <c r="B38" s="23"/>
       <c r="C38" s="23"/>
@@ -23656,7 +23656,7 @@
       <c r="R38" s="23"/>
       <c r="S38" s="23"/>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A39" s="23"/>
       <c r="B39" s="23"/>
       <c r="C39" s="23"/>
@@ -23677,7 +23677,7 @@
       <c r="R39" s="23"/>
       <c r="S39" s="23"/>
     </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A40" s="23"/>
       <c r="B40" s="23"/>
       <c r="C40" s="23"/>
@@ -23698,7 +23698,7 @@
       <c r="R40" s="23"/>
       <c r="S40" s="23"/>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A41" s="23"/>
       <c r="B41" s="23"/>
       <c r="C41" s="23"/>
@@ -23719,7 +23719,7 @@
       <c r="R41" s="23"/>
       <c r="S41" s="23"/>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A42" s="23"/>
       <c r="B42" s="23"/>
       <c r="C42" s="23"/>
@@ -23740,7 +23740,7 @@
       <c r="R42" s="23"/>
       <c r="S42" s="23"/>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A43" s="23"/>
       <c r="B43" s="23"/>
       <c r="C43" s="23"/>
@@ -23761,7 +23761,7 @@
       <c r="R43" s="23"/>
       <c r="S43" s="23"/>
     </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A44" s="23"/>
       <c r="B44" s="23"/>
       <c r="C44" s="23"/>
@@ -23782,7 +23782,7 @@
       <c r="R44" s="23"/>
       <c r="S44" s="23"/>
     </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A45" s="23"/>
       <c r="B45" s="23"/>
       <c r="C45" s="23"/>
@@ -23803,7 +23803,7 @@
       <c r="R45" s="23"/>
       <c r="S45" s="23"/>
     </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A46" s="23"/>
       <c r="B46" s="23"/>
       <c r="C46" s="23"/>
@@ -23824,7 +23824,7 @@
       <c r="R46" s="23"/>
       <c r="S46" s="23"/>
     </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A47" s="23"/>
       <c r="B47" s="23"/>
       <c r="C47" s="23"/>
@@ -23845,7 +23845,7 @@
       <c r="R47" s="23"/>
       <c r="S47" s="23"/>
     </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A48" s="23"/>
       <c r="B48" s="23"/>
       <c r="C48" s="23"/>
@@ -23866,7 +23866,7 @@
       <c r="R48" s="23"/>
       <c r="S48" s="23"/>
     </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A49" s="23"/>
       <c r="B49" s="23"/>
       <c r="C49" s="23"/>
@@ -23887,7 +23887,7 @@
       <c r="R49" s="23"/>
       <c r="S49" s="23"/>
     </row>
-    <row r="50" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A50" s="23"/>
       <c r="B50" s="23"/>
       <c r="C50" s="23"/>
@@ -23908,7 +23908,7 @@
       <c r="R50" s="23"/>
       <c r="S50" s="23"/>
     </row>
-    <row r="51" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A51" s="23"/>
       <c r="B51" s="23"/>
       <c r="C51" s="23"/>
@@ -23929,7 +23929,7 @@
       <c r="R51" s="23"/>
       <c r="S51" s="23"/>
     </row>
-    <row r="52" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A52" s="23"/>
       <c r="B52" s="23"/>
       <c r="C52" s="23"/>
@@ -23950,7 +23950,7 @@
       <c r="R52" s="23"/>
       <c r="S52" s="23"/>
     </row>
-    <row r="53" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A53" s="23"/>
       <c r="B53" s="23"/>
       <c r="C53" s="23"/>
@@ -23971,7 +23971,7 @@
       <c r="R53" s="23"/>
       <c r="S53" s="23"/>
     </row>
-    <row r="54" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A54" s="23"/>
       <c r="B54" s="23"/>
       <c r="C54" s="23"/>
@@ -23992,7 +23992,7 @@
       <c r="R54" s="23"/>
       <c r="S54" s="23"/>
     </row>
-    <row r="55" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A55" s="23"/>
       <c r="B55" s="23"/>
       <c r="C55" s="23"/>
@@ -24013,7 +24013,7 @@
       <c r="R55" s="23"/>
       <c r="S55" s="23"/>
     </row>
-    <row r="56" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A56" s="23"/>
       <c r="B56" s="23"/>
       <c r="C56" s="23"/>
@@ -24034,7 +24034,7 @@
       <c r="R56" s="23"/>
       <c r="S56" s="23"/>
     </row>
-    <row r="57" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A57" s="23"/>
       <c r="B57" s="23"/>
       <c r="C57" s="23"/>
@@ -24055,7 +24055,7 @@
       <c r="R57" s="23"/>
       <c r="S57" s="23"/>
     </row>
-    <row r="58" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A58" s="23"/>
       <c r="B58" s="23"/>
       <c r="C58" s="23"/>
@@ -24076,7 +24076,7 @@
       <c r="R58" s="23"/>
       <c r="S58" s="23"/>
     </row>
-    <row r="59" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A59" s="23"/>
       <c r="B59" s="23"/>
       <c r="C59" s="23"/>
@@ -24097,7 +24097,7 @@
       <c r="R59" s="23"/>
       <c r="S59" s="23"/>
     </row>
-    <row r="60" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A60" s="23"/>
       <c r="B60" s="23"/>
       <c r="C60" s="23"/>
@@ -24118,7 +24118,7 @@
       <c r="R60" s="23"/>
       <c r="S60" s="23"/>
     </row>
-    <row r="61" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A61" s="23"/>
       <c r="B61" s="23"/>
       <c r="C61" s="23"/>
@@ -24139,7 +24139,7 @@
       <c r="R61" s="23"/>
       <c r="S61" s="23"/>
     </row>
-    <row r="62" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A62" s="23"/>
       <c r="B62" s="23"/>
       <c r="C62" s="23"/>
@@ -24160,7 +24160,7 @@
       <c r="R62" s="23"/>
       <c r="S62" s="23"/>
     </row>
-    <row r="63" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A63" s="23"/>
       <c r="B63" s="23"/>
       <c r="C63" s="23"/>
@@ -24181,7 +24181,7 @@
       <c r="R63" s="23"/>
       <c r="S63" s="23"/>
     </row>
-    <row r="64" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A64" s="23"/>
       <c r="B64" s="23"/>
       <c r="C64" s="23"/>
@@ -24202,7 +24202,7 @@
       <c r="R64" s="23"/>
       <c r="S64" s="23"/>
     </row>
-    <row r="65" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A65" s="23"/>
       <c r="B65" s="23"/>
       <c r="C65" s="23"/>
@@ -24223,7 +24223,7 @@
       <c r="R65" s="23"/>
       <c r="S65" s="23"/>
     </row>
-    <row r="66" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A66" s="23"/>
       <c r="B66" s="23"/>
       <c r="C66" s="23"/>
@@ -24244,7 +24244,7 @@
       <c r="R66" s="23"/>
       <c r="S66" s="23"/>
     </row>
-    <row r="67" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A67" s="23"/>
       <c r="B67" s="23"/>
       <c r="C67" s="23"/>
@@ -24265,7 +24265,7 @@
       <c r="R67" s="23"/>
       <c r="S67" s="23"/>
     </row>
-    <row r="68" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A68" s="23"/>
       <c r="B68" s="23"/>
       <c r="C68" s="23"/>
@@ -24286,7 +24286,7 @@
       <c r="R68" s="23"/>
       <c r="S68" s="23"/>
     </row>
-    <row r="69" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A69" s="23"/>
       <c r="B69" s="23"/>
       <c r="C69" s="23"/>
@@ -24307,7 +24307,7 @@
       <c r="R69" s="23"/>
       <c r="S69" s="23"/>
     </row>
-    <row r="70" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A70" s="23"/>
       <c r="B70" s="23"/>
       <c r="C70" s="23"/>
@@ -24328,7 +24328,7 @@
       <c r="R70" s="23"/>
       <c r="S70" s="23"/>
     </row>
-    <row r="71" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A71" s="23"/>
       <c r="B71" s="23"/>
       <c r="C71" s="23"/>
@@ -24381,11 +24381,11 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="70.6640625" customWidth="1"/>
-    <col min="2" max="2" width="3.6640625" customWidth="1"/>
-    <col min="3" max="3" width="70.6640625" customWidth="1"/>
+    <col min="1" max="1" width="70.7109375" customWidth="1"/>
+    <col min="2" max="2" width="3.7109375" customWidth="1"/>
+    <col min="3" max="3" width="70.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="50.1" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
@@ -24393,7 +24393,7 @@
       <c r="B1" s="91"/>
       <c r="C1" s="91"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="92" t="s">
         <v>98</v>
       </c>
@@ -24402,7 +24402,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>0</v>
       </c>
@@ -24411,12 +24411,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A4" s="159"/>
       <c r="B4" s="159"/>
       <c r="C4" s="159"/>
     </row>
-    <row r="5" spans="1:3" ht="39.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A5" s="96" t="s">
         <v>100</v>
       </c>
@@ -24425,12 +24425,12 @@
         <v>101</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A6" s="95"/>
       <c r="B6" s="97"/>
       <c r="C6" s="99"/>
     </row>
-    <row r="7" spans="1:3" ht="65.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" ht="65.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="96" t="s">
         <v>160</v>
       </c>
@@ -24439,26 +24439,26 @@
         <v>169</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="101"/>
       <c r="B8" s="100"/>
       <c r="C8" s="102"/>
     </row>
-    <row r="9" spans="1:3" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A9" s="96" t="s">
-        <v>181</v>
+        <v>175</v>
       </c>
       <c r="B9" s="100"/>
       <c r="C9" s="98" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="15" x14ac:dyDescent="0.25">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="101"/>
       <c r="B10" s="100"/>
       <c r="C10" s="102"/>
     </row>
-    <row r="11" spans="1:3" ht="52.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" ht="51" x14ac:dyDescent="0.25">
       <c r="A11" s="96" t="s">
         <v>102</v>
       </c>
@@ -24467,12 +24467,12 @@
         <v>103</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A12" s="95"/>
       <c r="B12" s="97"/>
       <c r="C12" s="99"/>
     </row>
-    <row r="13" spans="1:3" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A13" s="96" t="s">
         <v>104</v>
       </c>
@@ -24481,12 +24481,12 @@
         <v>105</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A14" s="101"/>
       <c r="B14" s="100"/>
       <c r="C14" s="102"/>
     </row>
-    <row r="15" spans="1:3" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A15" s="96" t="s">
         <v>106</v>
       </c>
@@ -24495,12 +24495,12 @@
         <v>107</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A16" s="95"/>
       <c r="B16" s="97"/>
       <c r="C16" s="99"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="96" t="s">
         <v>108</v>
       </c>
@@ -24509,12 +24509,12 @@
         <v>109</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A18" s="95"/>
       <c r="B18" s="97"/>
       <c r="C18" s="99"/>
     </row>
-    <row r="19" spans="1:3" ht="26.4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A19" s="96" t="s">
         <v>110</v>
       </c>
@@ -24523,12 +24523,12 @@
         <v>111</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" ht="14.45" x14ac:dyDescent="0.3">
       <c r="A20" s="160"/>
       <c r="B20" s="160"/>
       <c r="C20" s="160"/>
     </row>
-    <row r="21" spans="1:3" ht="53.4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" ht="51.75" x14ac:dyDescent="0.25">
       <c r="A21" s="132" t="s">
         <v>161</v>
       </c>
@@ -24537,12 +24537,12 @@
         <v>162</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="23"/>
       <c r="B22" s="161"/>
       <c r="C22" s="23"/>
     </row>
-    <row r="23" spans="1:3" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" ht="39" x14ac:dyDescent="0.25">
       <c r="A23" s="134" t="s">
         <v>163</v>
       </c>
@@ -24551,12 +24551,12 @@
         <v>164</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="23"/>
       <c r="B24" s="161"/>
       <c r="C24" s="23"/>
     </row>
-    <row r="25" spans="1:3" ht="40.200000000000003" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" ht="39" x14ac:dyDescent="0.25">
       <c r="A25" s="132" t="s">
         <v>165</v>
       </c>
@@ -24565,7 +24565,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="23"/>
       <c r="B26" s="161"/>
       <c r="C26" s="23"/>

</xml_diff>